<commit_message>
Update estimates and macro shock employment
</commit_message>
<xml_diff>
--- a/input/reg_RMSE.xlsx
+++ b/input/reg_RMSE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA14B9C-2A05-4D78-A732-93217EE2FA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B48E2B-B07B-4C3F-B828-427C268AC08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-83" yWindow="0" windowWidth="14566" windowHeight="17363" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -828,7 +828,7 @@
         <v>18</v>
       </c>
       <c r="B2">
-        <v>0.74221509613052516</v>
+        <v>0.77710092075167148</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -836,7 +836,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>0.71708781548177403</v>
+        <v>0.80966819962611325</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -844,7 +844,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>0.39061084223695713</v>
+        <v>0.40685676867032922</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -852,7 +852,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0.46531245128873866</v>
+        <v>0.48603505601304164</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -860,7 +860,7 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1.0366469600587009</v>
+        <v>1.0366294171387864</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -868,7 +868,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>1.0148370111449538</v>
+        <v>1.0108885888661292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>